<commit_message>
Cleaned up the code, moved power computation to before downsampling
</commit_message>
<xml_diff>
--- a/Quantized_Filter_Coefficients.xlsx
+++ b/Quantized_Filter_Coefficients.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="41">
   <si>
-    <t xml:space="preserve">Filter Coefficients in Double precision Floating point </t>
+    <t xml:space="preserve">Filter Coefficients in Double precision Floating point (normalized to have energy 1)</t>
   </si>
   <si>
     <t xml:space="preserve">12 bit filter coefficients, with 1 bit for sign, 2 bits for integer and 9 bits for fractional part</t>
@@ -250,7 +250,7 @@
   <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G72" activeCellId="0" sqref="G72"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>